<commit_message>
fix col names in code and templates to match xlsx
</commit_message>
<xml_diff>
--- a/public/ead_template.xlsx
+++ b/public/ead_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21105"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="700" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1440" yWindow="3500" windowWidth="33160" windowHeight="16340" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PartI" sheetId="1" r:id="rId1"/>
@@ -98,6 +98,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -158,7 +161,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -170,6 +173,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -593,10 +597,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -647,6 +651,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="F5" s="1"/>
+      <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="F6" s="1"/>
@@ -723,15 +728,12 @@
     <row r="30" spans="6:6">
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="6:6">
-      <c r="F31" s="1"/>
-    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B30">
       <formula1>"class, collection, file, fonds, item, otherlevel, recordgrp, series, subfonds, subgrp, subseries"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E30">
       <formula1>"box, folder, box-folder, carton, reel, frame, reel-frame, volume, folio, page, sleeve, oversize, map-case, drawer"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
fixed 2 sheet code, found a bug in escape
</commit_message>
<xml_diff>
--- a/public/ead_template.xlsx
+++ b/public/ead_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21105"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="3500" windowWidth="33160" windowHeight="16340" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2520" yWindow="1640" windowWidth="33160" windowHeight="16340" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PartI" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>physloc</t>
   </si>
@@ -70,28 +70,25 @@
     <t>use_restrict</t>
   </si>
   <si>
-    <t>collection_date</t>
-  </si>
-  <si>
-    <t>c_level</t>
-  </si>
-  <si>
     <t>arrangement</t>
   </si>
   <si>
     <t>process_info</t>
   </si>
   <si>
-    <t>acq_info</t>
-  </si>
-  <si>
-    <t>related_mats</t>
-  </si>
-  <si>
     <t>c_num</t>
   </si>
   <si>
     <t>creator</t>
+  </si>
+  <si>
+    <t>collection date</t>
+  </si>
+  <si>
+    <t>acqinfo</t>
+  </si>
+  <si>
+    <t>c0x level</t>
   </si>
 </sst>
 </file>
@@ -513,25 +510,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8.5" customWidth="1"/>
-    <col min="2" max="14" width="13.6640625" customWidth="1"/>
-    <col min="17" max="17" width="67.83203125" customWidth="1"/>
-    <col min="18" max="18" width="21" customWidth="1"/>
-    <col min="19" max="19" width="13.6640625" customWidth="1"/>
-    <col min="20" max="20" width="10.83203125" style="1"/>
-    <col min="21" max="21" width="16.83203125" customWidth="1"/>
-    <col min="22" max="22" width="56.83203125" customWidth="1"/>
+    <col min="2" max="13" width="13.6640625" customWidth="1"/>
+    <col min="16" max="16" width="67.83203125" customWidth="1"/>
+    <col min="17" max="17" width="21" customWidth="1"/>
+    <col min="18" max="18" width="13.6640625" customWidth="1"/>
+    <col min="19" max="19" width="10.83203125" style="1"/>
+    <col min="20" max="20" width="16.83203125" customWidth="1"/>
+    <col min="21" max="21" width="56.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1">
+    <row r="1" spans="1:19" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -539,10 +536,10 @@
         <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>13</v>
@@ -554,10 +551,10 @@
         <v>15</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>7</v>
@@ -566,22 +563,19 @@
         <v>11</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="T1" s="3"/>
+      <c r="S1" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S3:S1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:R1048576">
       <formula1>"box, folder, box-folder, carton, reel, frame, reel-frame, volume, folio, page, sleeve, oversize, map-case, drawer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3:P1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O3:O1048576">
       <formula1>"class, collection, file, fonds, item, otherlevel, recordgrp, series, subfonds, subgrp, subseries"</formula1>
     </dataValidation>
   </dataValidations>
@@ -600,12 +594,14 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="10" width="18" customWidth="1"/>
+    <col min="1" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="18" style="1" customWidth="1"/>
+    <col min="5" max="10" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -613,12 +609,12 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -634,7 +630,7 @@
         <v>1</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>0</v>

</xml_diff>